<commit_message>
shipping option added to add more sevices
</commit_message>
<xml_diff>
--- a/public/uploads/bps/hd-leve.xlsx
+++ b/public/uploads/bps/hd-leve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hercoff-my.sharepoint.com/personal/marcio_freitas_hercoinc_com/Documents/Marcio/2010_AAAA_All_Files/2020 HD Custo Tabelas Saq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu18.04\var\www\hd-v2\public\uploads\bps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BA0334D-E2CF-484B-B902-A0A43D2FAC6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDE05E3-0DEA-422E-A471-599BCDBC1037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74DCA728-9E44-437A-A410-592AA8629A73}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{74DCA728-9E44-437A-A410-592AA8629A73}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">BPS </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>LEVE</t>
   </si>
@@ -434,26 +423,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D70"/>
+  <dimension ref="A2:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100</v>
       </c>
@@ -461,13 +447,10 @@
         <v>100</v>
       </c>
       <c r="C3" s="1">
-        <v>13.287000000000001</v>
-      </c>
-      <c r="D3" s="1">
         <v>10.094000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>200</v>
       </c>
@@ -475,13 +458,10 @@
         <v>200</v>
       </c>
       <c r="C4" s="1">
-        <v>13.7402</v>
-      </c>
-      <c r="D4" s="1">
         <v>10.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>300</v>
       </c>
@@ -489,13 +469,10 @@
         <v>300</v>
       </c>
       <c r="C5" s="1">
-        <v>15.2028</v>
-      </c>
-      <c r="D5" s="1">
         <v>10.505999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>400</v>
       </c>
@@ -503,13 +480,10 @@
         <v>400</v>
       </c>
       <c r="C6" s="1">
-        <v>15.2028</v>
-      </c>
-      <c r="D6" s="1">
         <v>10.711999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>500</v>
       </c>
@@ -517,13 +491,10 @@
         <v>500</v>
       </c>
       <c r="C7" s="1">
-        <v>18.7666</v>
-      </c>
-      <c r="D7" s="1">
         <v>11.618400000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>600</v>
       </c>
@@ -531,13 +502,10 @@
         <v>600</v>
       </c>
       <c r="C8" s="1">
-        <v>18.7666</v>
-      </c>
-      <c r="D8" s="1">
         <v>11.824400000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>700</v>
       </c>
@@ -545,13 +513,10 @@
         <v>700</v>
       </c>
       <c r="C9" s="1">
-        <v>18.7666</v>
-      </c>
-      <c r="D9" s="1">
         <v>12.0304</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>800</v>
       </c>
@@ -559,13 +524,10 @@
         <v>800</v>
       </c>
       <c r="C10" s="1">
-        <v>18.7666</v>
-      </c>
-      <c r="D10" s="1">
         <v>12.236400000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>900</v>
       </c>
@@ -573,13 +535,10 @@
         <v>900</v>
       </c>
       <c r="C11" s="1">
-        <v>18.7666</v>
-      </c>
-      <c r="D11" s="1">
         <v>12.442399999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1000</v>
       </c>
@@ -587,13 +546,10 @@
         <v>1000</v>
       </c>
       <c r="C12" s="1">
-        <v>25.317399999999999</v>
-      </c>
-      <c r="D12" s="1">
         <v>13.359099999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1500</v>
       </c>
@@ -601,13 +557,10 @@
         <v>1500</v>
       </c>
       <c r="C13" s="1">
-        <v>25.317399999999999</v>
-      </c>
-      <c r="D13" s="1">
         <v>15.089500000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2000</v>
       </c>
@@ -615,13 +568,10 @@
         <v>2000</v>
       </c>
       <c r="C14" s="1">
-        <v>31.106000000000002</v>
-      </c>
-      <c r="D14" s="1">
         <v>16.830200000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2500</v>
       </c>
@@ -629,13 +579,10 @@
         <v>2500</v>
       </c>
       <c r="C15" s="1">
-        <v>31.106000000000002</v>
-      </c>
-      <c r="D15" s="1">
         <v>18.560600000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3000</v>
       </c>
@@ -643,13 +590,10 @@
         <v>3000</v>
       </c>
       <c r="C16" s="1">
-        <v>36.626800000000003</v>
-      </c>
-      <c r="D16" s="1">
         <v>20.301300000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3500</v>
       </c>
@@ -657,13 +601,10 @@
         <v>3500</v>
       </c>
       <c r="C17" s="1">
-        <v>36.626800000000003</v>
-      </c>
-      <c r="D17" s="1">
         <v>22.031700000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4000</v>
       </c>
@@ -671,13 +612,10 @@
         <v>4000</v>
       </c>
       <c r="C18" s="1">
-        <v>42.230000000000004</v>
-      </c>
-      <c r="D18" s="1">
         <v>23.772399999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4500</v>
       </c>
@@ -685,13 +623,10 @@
         <v>4500</v>
       </c>
       <c r="C19" s="1">
-        <v>42.230000000000004</v>
-      </c>
-      <c r="D19" s="1">
         <v>25.502799999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5000</v>
       </c>
@@ -699,13 +634,10 @@
         <v>5000</v>
       </c>
       <c r="C20" s="1">
-        <v>48.801400000000001</v>
-      </c>
-      <c r="D20" s="1">
         <v>27.367100000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5500</v>
       </c>
@@ -713,13 +645,10 @@
         <v>5.5</v>
       </c>
       <c r="C21" s="1">
-        <v>48.801400000000001</v>
-      </c>
-      <c r="D21" s="1">
         <v>29.231400000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>6000</v>
       </c>
@@ -727,13 +656,10 @@
         <v>6</v>
       </c>
       <c r="C22" s="1">
-        <v>55.424300000000002</v>
-      </c>
-      <c r="D22" s="1">
         <v>31.095700000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6500</v>
       </c>
@@ -741,13 +667,10 @@
         <v>6.5</v>
       </c>
       <c r="C23" s="1">
-        <v>55.424300000000002</v>
-      </c>
-      <c r="D23" s="1">
         <v>32.96</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7000</v>
       </c>
@@ -755,13 +678,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="1">
-        <v>61.964799999999997</v>
-      </c>
-      <c r="D24" s="1">
         <v>34.824300000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>7500</v>
       </c>
@@ -769,13 +689,10 @@
         <v>7.5</v>
       </c>
       <c r="C25" s="1">
-        <v>61.964799999999997</v>
-      </c>
-      <c r="D25" s="1">
         <v>36.688600000000008</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8000</v>
       </c>
@@ -783,13 +700,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="1">
-        <v>67.743100000000013</v>
-      </c>
-      <c r="D26" s="1">
         <v>38.552900000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8500</v>
       </c>
@@ -797,13 +711,10 @@
         <v>8.5</v>
       </c>
       <c r="C27" s="1">
-        <v>67.743100000000013</v>
-      </c>
-      <c r="D27" s="1">
         <v>40.417199999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9000</v>
       </c>
@@ -811,13 +722,10 @@
         <v>9</v>
       </c>
       <c r="C28" s="1">
-        <v>73.1815</v>
-      </c>
-      <c r="D28" s="1">
         <v>42.281499999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>9500</v>
       </c>
@@ -825,13 +733,10 @@
         <v>9.5</v>
       </c>
       <c r="C29" s="1">
-        <v>73.1815</v>
-      </c>
-      <c r="D29" s="1">
         <v>44.145800000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10000</v>
       </c>
@@ -839,13 +744,10 @@
         <v>10</v>
       </c>
       <c r="C30" s="1">
-        <v>79.855900000000005</v>
-      </c>
-      <c r="D30" s="1">
         <v>46.010099999999994</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10500</v>
       </c>
@@ -853,13 +755,10 @@
         <v>10.5</v>
       </c>
       <c r="C31" s="1">
-        <v>79.855900000000005</v>
-      </c>
-      <c r="D31" s="1">
         <v>47.874399999999987</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>11000</v>
       </c>
@@ -867,13 +766,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="1">
-        <v>86.530300000000011</v>
-      </c>
-      <c r="D32" s="1">
         <v>49.738699999999994</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>11500</v>
       </c>
@@ -881,13 +777,10 @@
         <v>11.5</v>
       </c>
       <c r="C33" s="1">
-        <v>86.530300000000011</v>
-      </c>
-      <c r="D33" s="1">
         <v>51.602999999999994</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>12000</v>
       </c>
@@ -895,13 +788,10 @@
         <v>12</v>
       </c>
       <c r="C34" s="1">
-        <v>93.204700000000017</v>
-      </c>
-      <c r="D34" s="1">
         <v>53.467299999999987</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12500</v>
       </c>
@@ -909,13 +799,10 @@
         <v>12.5</v>
       </c>
       <c r="C35" s="1">
-        <v>93.204700000000017</v>
-      </c>
-      <c r="D35" s="1">
         <v>55.331599999999987</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>13000</v>
       </c>
@@ -923,13 +810,10 @@
         <v>13</v>
       </c>
       <c r="C36" s="1">
-        <v>99.879100000000022</v>
-      </c>
-      <c r="D36" s="1">
         <v>57.195899999999988</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>13500</v>
       </c>
@@ -937,13 +821,10 @@
         <v>13.5</v>
       </c>
       <c r="C37" s="1">
-        <v>99.879100000000022</v>
-      </c>
-      <c r="D37" s="1">
         <v>59.060199999999988</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>14000</v>
       </c>
@@ -951,13 +832,10 @@
         <v>14</v>
       </c>
       <c r="C38" s="1">
-        <v>106.55350000000001</v>
-      </c>
-      <c r="D38" s="1">
         <v>60.924499999999981</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>14500</v>
       </c>
@@ -965,13 +843,10 @@
         <v>14.5</v>
       </c>
       <c r="C39" s="1">
-        <v>106.55350000000001</v>
-      </c>
-      <c r="D39" s="1">
         <v>62.788799999999981</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>15000</v>
       </c>
@@ -979,13 +854,10 @@
         <v>15</v>
       </c>
       <c r="C40" s="1">
-        <v>113.22790000000002</v>
-      </c>
-      <c r="D40" s="1">
         <v>64.653099999999981</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>15500</v>
       </c>
@@ -993,13 +865,10 @@
         <v>15.5</v>
       </c>
       <c r="C41" s="1">
-        <v>113.22790000000002</v>
-      </c>
-      <c r="D41" s="1">
         <v>66.517399999999981</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>16000</v>
       </c>
@@ -1007,13 +876,10 @@
         <v>16</v>
       </c>
       <c r="C42" s="1">
-        <v>119.90230000000003</v>
-      </c>
-      <c r="D42" s="1">
         <v>68.381699999999981</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>16500</v>
       </c>
@@ -1021,13 +887,10 @@
         <v>16.5</v>
       </c>
       <c r="C43" s="1">
-        <v>119.90230000000003</v>
-      </c>
-      <c r="D43" s="1">
         <v>70.245999999999981</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>17000</v>
       </c>
@@ -1035,13 +898,10 @@
         <v>17</v>
       </c>
       <c r="C44" s="1">
-        <v>126.57670000000003</v>
-      </c>
-      <c r="D44" s="1">
         <v>72.110299999999981</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>17500</v>
       </c>
@@ -1049,13 +909,10 @@
         <v>17.5</v>
       </c>
       <c r="C45" s="1">
-        <v>126.57670000000003</v>
-      </c>
-      <c r="D45" s="1">
         <v>73.974599999999981</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>18000</v>
       </c>
@@ -1063,13 +920,10 @@
         <v>18</v>
       </c>
       <c r="C46" s="1">
-        <v>133.25110000000004</v>
-      </c>
-      <c r="D46" s="1">
         <v>75.838899999999981</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>18500</v>
       </c>
@@ -1077,13 +931,10 @@
         <v>18.5</v>
       </c>
       <c r="C47" s="1">
-        <v>133.25110000000004</v>
-      </c>
-      <c r="D47" s="1">
         <v>77.703199999999981</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>19000</v>
       </c>
@@ -1091,13 +942,10 @@
         <v>19</v>
       </c>
       <c r="C48" s="1">
-        <v>139.92550000000003</v>
-      </c>
-      <c r="D48" s="1">
         <v>79.567499999999981</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>19500</v>
       </c>
@@ -1105,13 +953,10 @@
         <v>19.5</v>
       </c>
       <c r="C49" s="1">
-        <v>139.92550000000003</v>
-      </c>
-      <c r="D49" s="1">
         <v>81.431799999999981</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>20000</v>
       </c>
@@ -1119,13 +964,10 @@
         <v>20</v>
       </c>
       <c r="C50" s="1">
-        <v>146.59990000000002</v>
-      </c>
-      <c r="D50" s="1">
         <v>83.296099999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>20500</v>
       </c>
@@ -1133,13 +975,10 @@
         <v>20.5</v>
       </c>
       <c r="C51" s="1">
-        <v>146.59990000000002</v>
-      </c>
-      <c r="D51" s="1">
         <v>85.160399999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>21000</v>
       </c>
@@ -1147,13 +986,10 @@
         <v>21</v>
       </c>
       <c r="C52" s="1">
-        <v>153.27430000000001</v>
-      </c>
-      <c r="D52" s="1">
         <v>87.024699999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>21500</v>
       </c>
@@ -1161,13 +997,10 @@
         <v>21.5</v>
       </c>
       <c r="C53" s="1">
-        <v>153.27430000000001</v>
-      </c>
-      <c r="D53" s="1">
         <v>88.888999999999996</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>22000</v>
       </c>
@@ -1175,13 +1008,10 @@
         <v>22</v>
       </c>
       <c r="C54" s="1">
-        <v>159.9487</v>
-      </c>
-      <c r="D54" s="1">
         <v>90.753299999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>22500</v>
       </c>
@@ -1189,13 +1019,10 @@
         <v>22.5</v>
       </c>
       <c r="C55" s="1">
-        <v>159.9487</v>
-      </c>
-      <c r="D55" s="1">
         <v>92.617599999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>23000</v>
       </c>
@@ -1203,13 +1030,10 @@
         <v>23</v>
       </c>
       <c r="C56" s="1">
-        <v>166.62309999999999</v>
-      </c>
-      <c r="D56" s="1">
         <v>94.48190000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>23500</v>
       </c>
@@ -1217,13 +1041,10 @@
         <v>23.5</v>
       </c>
       <c r="C57" s="1">
-        <v>166.62309999999999</v>
-      </c>
-      <c r="D57" s="1">
         <v>96.34620000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>24000</v>
       </c>
@@ -1231,13 +1052,10 @@
         <v>24</v>
       </c>
       <c r="C58" s="1">
-        <v>173.29749999999999</v>
-      </c>
-      <c r="D58" s="1">
         <v>98.21050000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>24500</v>
       </c>
@@ -1245,13 +1063,10 @@
         <v>24.5</v>
       </c>
       <c r="C59" s="1">
-        <v>173.29749999999999</v>
-      </c>
-      <c r="D59" s="1">
         <v>100.07480000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>25000</v>
       </c>
@@ -1259,13 +1074,10 @@
         <v>25</v>
       </c>
       <c r="C60" s="1">
-        <v>179.97189999999998</v>
-      </c>
-      <c r="D60" s="1">
         <v>101.93910000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>25500</v>
       </c>
@@ -1273,13 +1085,10 @@
         <v>25.5</v>
       </c>
       <c r="C61" s="1">
-        <v>179.97189999999998</v>
-      </c>
-      <c r="D61" s="1">
         <v>103.80340000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>26000</v>
       </c>
@@ -1287,13 +1096,10 @@
         <v>26</v>
       </c>
       <c r="C62" s="1">
-        <v>186.64629999999997</v>
-      </c>
-      <c r="D62" s="1">
         <v>105.66770000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>26500</v>
       </c>
@@ -1301,13 +1107,10 @@
         <v>26.5</v>
       </c>
       <c r="C63" s="1">
-        <v>186.64629999999997</v>
-      </c>
-      <c r="D63" s="1">
         <v>107.53200000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>27000</v>
       </c>
@@ -1315,13 +1118,10 @@
         <v>27</v>
       </c>
       <c r="C64" s="1">
-        <v>193.32069999999993</v>
-      </c>
-      <c r="D64" s="1">
         <v>109.39630000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>27500</v>
       </c>
@@ -1329,13 +1129,10 @@
         <v>27.5</v>
       </c>
       <c r="C65" s="1">
-        <v>193.32069999999993</v>
-      </c>
-      <c r="D65" s="1">
         <v>111.26060000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>28000</v>
       </c>
@@ -1343,13 +1140,10 @@
         <v>28</v>
       </c>
       <c r="C66" s="1">
-        <v>199.99509999999992</v>
-      </c>
-      <c r="D66" s="1">
         <v>113.12490000000003</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>28500</v>
       </c>
@@ -1357,13 +1151,10 @@
         <v>28.5</v>
       </c>
       <c r="C67" s="1">
-        <v>199.99509999999992</v>
-      </c>
-      <c r="D67" s="1">
         <v>114.98920000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>29000</v>
       </c>
@@ -1371,13 +1162,10 @@
         <v>29</v>
       </c>
       <c r="C68" s="1">
-        <v>206.66949999999991</v>
-      </c>
-      <c r="D68" s="1">
         <v>116.85350000000003</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>29500</v>
       </c>
@@ -1385,13 +1173,10 @@
         <v>29.5</v>
       </c>
       <c r="C69" s="1">
-        <v>206.66949999999991</v>
-      </c>
-      <c r="D69" s="1">
         <v>118.71780000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>30000</v>
       </c>
@@ -1399,9 +1184,6 @@
         <v>30</v>
       </c>
       <c r="C70" s="1">
-        <v>213.34389999999991</v>
-      </c>
-      <c r="D70" s="1">
         <v>120.58210000000004</v>
       </c>
     </row>
@@ -1412,6 +1194,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CDA795DBB6F9A6458BF0B007205B2904" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="430d60cf902e72d61d125cab07fdec1b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1c7ad846-6561-4742-a254-da78342a384c" xmlns:ns4="f12da351-31bf-4af6-a5e0-5c610a8aab9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9ebab88c37af433c5fba9db951e3af99" ns3:_="" ns4:_="">
     <xsd:import namespace="1c7ad846-6561-4742-a254-da78342a384c"/>
@@ -1634,15 +1425,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1650,6 +1432,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5E1FF44-BB8E-4121-BCFF-CB2D4453A4C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28FDD389-9944-4F36-9797-77F6E1B11982}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1668,14 +1458,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5E1FF44-BB8E-4121-BCFF-CB2D4453A4C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{619E583B-C577-4BA3-9DB5-192A9FAC5709}">
   <ds:schemaRefs>

</xml_diff>